<commit_message>
Create two versions of a the  templates (stamped & unstamped)
</commit_message>
<xml_diff>
--- a/xls/March 2025 - Valuation 90.xlsx
+++ b/xls/March 2025 - Valuation 90.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>S/N</t>
   </si>
@@ -57,10 +57,6 @@
   </si>
   <si>
     <t>C22C</t>
-  </si>
-  <si>
-    <t>7, Ahidjo Ekun,
-Akure, Ondo – Nigeria.</t>
   </si>
   <si>
     <t>C22D</t>
@@ -77,7 +73,45 @@
     <t>Mr. Man James</t>
   </si>
   <si>
-    <t>Mrs. Woman Jobs</t>
+    <t>1 Bedroom 2-in-1 Bungalow</t>
+  </si>
+  <si>
+    <t>2 bedroom Semi-detached Bungalow</t>
+  </si>
+  <si>
+    <t>3 bedroom Semi-detached Bungalow</t>
+  </si>
+  <si>
+    <t>4 bedroom detached bungalow</t>
+  </si>
+  <si>
+    <t>4 bedroom detached luxury bungalow</t>
+  </si>
+  <si>
+    <t>Mrs. Woman Jobs 1</t>
+  </si>
+  <si>
+    <t>Mrs. Woman Jobs 2</t>
+  </si>
+  <si>
+    <t>Mrs. Woman Jobs 3</t>
+  </si>
+  <si>
+    <t>Mrs. Woman Jobs 4</t>
+  </si>
+  <si>
+    <t>Mrs. Woman Jobs 5</t>
+  </si>
+  <si>
+    <t>Mrs. Woman Jobs 6</t>
+  </si>
+  <si>
+    <t>1 Bedroom 8-in-1 Flat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+7, Ahidjo Ekun,
+Akure, Ondo – Nigeria.</t>
   </si>
 </sst>
 </file>
@@ -140,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -167,6 +201,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -383,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -406,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -432,10 +469,10 @@
         <v>36</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>7</v>
@@ -446,8 +483,8 @@
       <c r="F2" s="9">
         <v>6500000</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>10</v>
+      <c r="G2" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="H2" s="5">
         <v>814</v>
@@ -458,7 +495,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>8</v>
@@ -467,15 +504,145 @@
         <v>7</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="9">
         <v>6500000</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
+      <c r="G3" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="5">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>37</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9">
+        <v>6500000</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="5">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>37</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9">
+        <v>6500000</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="5">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>37</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9">
+        <v>6500000</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="5">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>37</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9">
+        <v>6500000</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="5">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>37</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9">
+        <v>6500000</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="5">
         <v>815</v>
       </c>
     </row>

</xml_diff>